<commit_message>
Mapped definitions to value sets
</commit_message>
<xml_diff>
--- a/IG-Publisher/output/StructureDefinition-Claim.xlsx
+++ b/IG-Publisher/output/StructureDefinition-Claim.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5152" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5152" uniqueCount="655">
   <si>
     <t>Path</t>
   </si>
@@ -991,7 +991,7 @@
     <t>The role codes for the care team members.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/claim-careteamrole</t>
+    <t>https://swasth-digital-health-foundation.github.io/standards/output/ValueSet-health-service-provider-role.html</t>
   </si>
   <si>
     <t>Claim.careTeam.qualification</t>
@@ -1316,7 +1316,7 @@
     <t>Example procedure type codes.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/ex-procedure-type</t>
+    <t>https://swasth-digital-health-foundation.github.io/standards/output/ValueSet-procedure-type-description.html</t>
   </si>
   <si>
     <t>Claim.procedure.date</t>
@@ -1347,10 +1347,10 @@
     <t>This identifies the actual clinical procedure.</t>
   </si>
   <si>
-    <t>Example ICD10 Procedure codes.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/icd-10-procedures</t>
+    <t>Procedure codes.</t>
+  </si>
+  <si>
+    <t>https://icd.who.int/browse10/2010/en</t>
   </si>
   <si>
     <t>Claim.procedure.udi</t>
@@ -1691,7 +1691,7 @@
     <t>Benefit categories such as: oral-basic, major, glasses.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/ex-benefitcategory</t>
+    <t>https://swasth-digital-health-foundation.github.io/standards/output/ValueSet-claim-service-categories.html</t>
   </si>
   <si>
     <t>Claim.item.productOrService</t>
@@ -1944,6 +1944,9 @@
   </si>
   <si>
     <t>Claim.item.detail.category</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/ex-benefitcategory</t>
   </si>
   <si>
     <t>Claim.item.detail.productOrService</t>
@@ -2212,7 +2215,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="121.30859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="52.02734375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="101.6875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
@@ -15876,7 +15879,7 @@
         <v>541</v>
       </c>
       <c r="Y126" t="s" s="2">
-        <v>542</v>
+        <v>625</v>
       </c>
       <c r="Z126" t="s" s="2">
         <v>42</v>
@@ -15920,7 +15923,7 @@
     </row>
     <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" t="s" s="2">
@@ -16004,7 +16007,7 @@
         <v>42</v>
       </c>
       <c r="AE127" t="s" s="2">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="AF127" t="s" s="2">
         <v>50</v>
@@ -16030,7 +16033,7 @@
     </row>
     <row r="128" hidden="true">
       <c r="A128" t="s" s="2">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" t="s" s="2">
@@ -16056,13 +16059,13 @@
         <v>126</v>
       </c>
       <c r="K128" t="s" s="2">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="L128" t="s" s="2">
         <v>553</v>
       </c>
       <c r="M128" t="s" s="2">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="N128" t="s" s="2">
         <v>555</v>
@@ -16114,7 +16117,7 @@
         <v>42</v>
       </c>
       <c r="AE128" t="s" s="2">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="AF128" t="s" s="2">
         <v>40</v>
@@ -16140,7 +16143,7 @@
     </row>
     <row r="129" hidden="true">
       <c r="A129" t="s" s="2">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" t="s" s="2">
@@ -16224,7 +16227,7 @@
         <v>42</v>
       </c>
       <c r="AE129" t="s" s="2">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="AF129" t="s" s="2">
         <v>40</v>
@@ -16250,7 +16253,7 @@
     </row>
     <row r="130" hidden="true">
       <c r="A130" t="s" s="2">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" t="s" s="2">
@@ -16332,7 +16335,7 @@
         <v>42</v>
       </c>
       <c r="AE130" t="s" s="2">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="AF130" t="s" s="2">
         <v>40</v>
@@ -16358,7 +16361,7 @@
     </row>
     <row r="131" hidden="true">
       <c r="A131" t="s" s="2">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" t="s" s="2">
@@ -16440,7 +16443,7 @@
         <v>42</v>
       </c>
       <c r="AE131" t="s" s="2">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="AF131" t="s" s="2">
         <v>40</v>
@@ -16466,7 +16469,7 @@
     </row>
     <row r="132" hidden="true">
       <c r="A132" t="s" s="2">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" t="s" s="2">
@@ -16550,7 +16553,7 @@
         <v>42</v>
       </c>
       <c r="AE132" t="s" s="2">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="AF132" t="s" s="2">
         <v>40</v>
@@ -16576,7 +16579,7 @@
     </row>
     <row r="133" hidden="true">
       <c r="A133" t="s" s="2">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B133" s="2"/>
       <c r="C133" t="s" s="2">
@@ -16660,7 +16663,7 @@
         <v>42</v>
       </c>
       <c r="AE133" t="s" s="2">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="AF133" t="s" s="2">
         <v>40</v>
@@ -16686,7 +16689,7 @@
     </row>
     <row r="134" hidden="true">
       <c r="A134" t="s" s="2">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" t="s" s="2">
@@ -16768,7 +16771,7 @@
         <v>42</v>
       </c>
       <c r="AE134" t="s" s="2">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="AF134" t="s" s="2">
         <v>40</v>
@@ -16794,7 +16797,7 @@
     </row>
     <row r="135" hidden="true">
       <c r="A135" t="s" s="2">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" t="s" s="2">
@@ -16876,7 +16879,7 @@
         <v>42</v>
       </c>
       <c r="AE135" t="s" s="2">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="AF135" t="s" s="2">
         <v>40</v>
@@ -16902,7 +16905,7 @@
     </row>
     <row r="136" hidden="true">
       <c r="A136" t="s" s="2">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" t="s" s="2">
@@ -17008,7 +17011,7 @@
     </row>
     <row r="137" hidden="true">
       <c r="A137" t="s" s="2">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B137" s="2"/>
       <c r="C137" t="s" s="2">
@@ -17116,7 +17119,7 @@
     </row>
     <row r="138" hidden="true">
       <c r="A138" t="s" s="2">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B138" s="2"/>
       <c r="C138" t="s" s="2">
@@ -17226,7 +17229,7 @@
     </row>
     <row r="139" hidden="true">
       <c r="A139" t="s" s="2">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" t="s" s="2">
@@ -17308,7 +17311,7 @@
         <v>42</v>
       </c>
       <c r="AE139" t="s" s="2">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="AF139" t="s" s="2">
         <v>50</v>
@@ -17334,7 +17337,7 @@
     </row>
     <row r="140" hidden="true">
       <c r="A140" t="s" s="2">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" t="s" s="2">
@@ -17416,7 +17419,7 @@
         <v>42</v>
       </c>
       <c r="AE140" t="s" s="2">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="AF140" t="s" s="2">
         <v>40</v>
@@ -17442,7 +17445,7 @@
     </row>
     <row r="141" hidden="true">
       <c r="A141" t="s" s="2">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" t="s" s="2">
@@ -17508,7 +17511,7 @@
         <v>541</v>
       </c>
       <c r="Y141" t="s" s="2">
-        <v>542</v>
+        <v>625</v>
       </c>
       <c r="Z141" t="s" s="2">
         <v>42</v>
@@ -17526,7 +17529,7 @@
         <v>42</v>
       </c>
       <c r="AE141" t="s" s="2">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="AF141" t="s" s="2">
         <v>40</v>
@@ -17552,7 +17555,7 @@
     </row>
     <row r="142" hidden="true">
       <c r="A142" t="s" s="2">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" t="s" s="2">
@@ -17636,7 +17639,7 @@
         <v>42</v>
       </c>
       <c r="AE142" t="s" s="2">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="AF142" t="s" s="2">
         <v>50</v>
@@ -17662,7 +17665,7 @@
     </row>
     <row r="143" hidden="true">
       <c r="A143" t="s" s="2">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" t="s" s="2">
@@ -17688,13 +17691,13 @@
         <v>126</v>
       </c>
       <c r="K143" t="s" s="2">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="L143" t="s" s="2">
         <v>553</v>
       </c>
       <c r="M143" t="s" s="2">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="N143" t="s" s="2">
         <v>555</v>
@@ -17746,7 +17749,7 @@
         <v>42</v>
       </c>
       <c r="AE143" t="s" s="2">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="AF143" t="s" s="2">
         <v>40</v>
@@ -17772,7 +17775,7 @@
     </row>
     <row r="144" hidden="true">
       <c r="A144" t="s" s="2">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" t="s" s="2">
@@ -17856,7 +17859,7 @@
         <v>42</v>
       </c>
       <c r="AE144" t="s" s="2">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="AF144" t="s" s="2">
         <v>40</v>
@@ -17882,7 +17885,7 @@
     </row>
     <row r="145" hidden="true">
       <c r="A145" t="s" s="2">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" t="s" s="2">
@@ -17964,7 +17967,7 @@
         <v>42</v>
       </c>
       <c r="AE145" t="s" s="2">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="AF145" t="s" s="2">
         <v>40</v>
@@ -17990,7 +17993,7 @@
     </row>
     <row r="146" hidden="true">
       <c r="A146" t="s" s="2">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" t="s" s="2">
@@ -18072,7 +18075,7 @@
         <v>42</v>
       </c>
       <c r="AE146" t="s" s="2">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="AF146" t="s" s="2">
         <v>40</v>
@@ -18098,7 +18101,7 @@
     </row>
     <row r="147" hidden="true">
       <c r="A147" t="s" s="2">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" t="s" s="2">
@@ -18182,7 +18185,7 @@
         <v>42</v>
       </c>
       <c r="AE147" t="s" s="2">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="AF147" t="s" s="2">
         <v>40</v>
@@ -18208,7 +18211,7 @@
     </row>
     <row r="148" hidden="true">
       <c r="A148" t="s" s="2">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" t="s" s="2">
@@ -18292,7 +18295,7 @@
         <v>42</v>
       </c>
       <c r="AE148" t="s" s="2">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="AF148" t="s" s="2">
         <v>40</v>
@@ -18318,7 +18321,7 @@
     </row>
     <row r="149" hidden="true">
       <c r="A149" t="s" s="2">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" t="s" s="2">
@@ -18400,7 +18403,7 @@
         <v>42</v>
       </c>
       <c r="AE149" t="s" s="2">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="AF149" t="s" s="2">
         <v>40</v>
@@ -18426,7 +18429,7 @@
     </row>
     <row r="150" hidden="true">
       <c r="A150" t="s" s="2">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" t="s" s="2">
@@ -18452,14 +18455,14 @@
         <v>582</v>
       </c>
       <c r="K150" t="s" s="2">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="L150" t="s" s="2">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="M150" s="2"/>
       <c r="N150" t="s" s="2">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="O150" t="s" s="2">
         <v>42</v>
@@ -18508,7 +18511,7 @@
         <v>42</v>
       </c>
       <c r="AE150" t="s" s="2">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="AF150" t="s" s="2">
         <v>40</v>

</xml_diff>